<commit_message>
update readme and data files -nodeployment
</commit_message>
<xml_diff>
--- a/data-migration/xlsx_1900-/1923_Winter.xlsx
+++ b/data-migration/xlsx_1900-/1923_Winter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\TEMP REPOSITORY\VVZ 1833-2014\_XLSX_2024-05-22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TEMP_REPOSITORY\VVZ 1833-2014\_XLSX_2024-05-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD576E6E-8F2E-48FF-BEF0-E95E2AD3AA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28097DE-4964-4C52-9E2F-9FF7929C29AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4138,9 +4138,6 @@
     <t>veraguth_o</t>
   </si>
   <si>
-    <t>silberschmidt _w</t>
-  </si>
-  <si>
     <t>gysi_a</t>
   </si>
   <si>
@@ -4186,15 +4183,9 @@
     <t>pfenninger_hf</t>
   </si>
   <si>
-    <t>frey_h</t>
-  </si>
-  <si>
     <t>brun_h</t>
   </si>
   <si>
-    <t>vonmonakow_c</t>
-  </si>
-  <si>
     <t>brun_r</t>
   </si>
   <si>
@@ -4210,9 +4201,6 @@
     <t>vonmonakow_p</t>
   </si>
   <si>
-    <t>meyerrueegg_h</t>
-  </si>
-  <si>
     <t>meyerwirz_e</t>
   </si>
   <si>
@@ -4222,9 +4210,6 @@
     <t>wehrli_ga</t>
   </si>
   <si>
-    <t>schinz_hr</t>
-  </si>
-  <si>
     <t>schinz_h</t>
   </si>
   <si>
@@ -4277,6 +4262,21 @@
   </si>
   <si>
     <t>nager_fr</t>
+  </si>
+  <si>
+    <t>frey_h2</t>
+  </si>
+  <si>
+    <t>meyer-rueegg_h</t>
+  </si>
+  <si>
+    <t>monakow_c</t>
+  </si>
+  <si>
+    <t>schinz_hr2</t>
+  </si>
+  <si>
+    <t>silberschmidt_w</t>
   </si>
 </sst>
 </file>
@@ -4318,11 +4318,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4626,11 +4629,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E157" workbookViewId="0">
-      <selection activeCell="H174" sqref="H174"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="34.21875" customWidth="1"/>
     <col min="6" max="6" width="30.88671875" customWidth="1"/>
@@ -4662,7 +4665,7 @@
         <v>1361</v>
       </c>
       <c r="I1" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4688,10 +4691,10 @@
         <v>1248</v>
       </c>
       <c r="I2" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J2" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -4717,10 +4720,10 @@
         <v>1248</v>
       </c>
       <c r="I3" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J3" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4746,7 +4749,7 @@
         <v>1362</v>
       </c>
       <c r="I4" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4772,7 +4775,7 @@
         <v>1362</v>
       </c>
       <c r="I5" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4798,7 +4801,7 @@
         <v>1363</v>
       </c>
       <c r="I6" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -4824,7 +4827,7 @@
         <v>1250</v>
       </c>
       <c r="I7" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -4850,7 +4853,7 @@
         <v>1250</v>
       </c>
       <c r="I8" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -4876,7 +4879,7 @@
         <v>1251</v>
       </c>
       <c r="I9" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -4902,7 +4905,7 @@
         <v>1362</v>
       </c>
       <c r="I10" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -4928,7 +4931,7 @@
         <v>1363</v>
       </c>
       <c r="I11" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4954,7 +4957,7 @@
         <v>1249</v>
       </c>
       <c r="I12" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -4980,7 +4983,7 @@
         <v>1249</v>
       </c>
       <c r="I13" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -5006,7 +5009,7 @@
         <v>1252</v>
       </c>
       <c r="I14" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -5032,7 +5035,7 @@
         <v>1363</v>
       </c>
       <c r="I15" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -5058,7 +5061,7 @@
         <v>1251</v>
       </c>
       <c r="I16" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -5084,10 +5087,10 @@
         <v>1248</v>
       </c>
       <c r="I17" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J17" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -5113,10 +5116,10 @@
         <v>1248</v>
       </c>
       <c r="I18" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J18" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -5142,7 +5145,7 @@
         <v>1363</v>
       </c>
       <c r="I19" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -5168,7 +5171,7 @@
         <v>1250</v>
       </c>
       <c r="I20" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -5194,7 +5197,7 @@
         <v>1249</v>
       </c>
       <c r="I21" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -5220,7 +5223,7 @@
         <v>1252</v>
       </c>
       <c r="I22" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -5246,7 +5249,7 @@
         <v>1363</v>
       </c>
       <c r="I23" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -5272,7 +5275,7 @@
         <v>1253</v>
       </c>
       <c r="I24" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -5298,7 +5301,7 @@
         <v>1254</v>
       </c>
       <c r="I25" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -5321,10 +5324,10 @@
         <v>958</v>
       </c>
       <c r="H26" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="I26" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5347,10 +5350,10 @@
         <v>959</v>
       </c>
       <c r="H27" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="I27" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5376,10 +5379,10 @@
         <v>1255</v>
       </c>
       <c r="I28" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J28" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -5405,7 +5408,7 @@
         <v>1256</v>
       </c>
       <c r="I29" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -5431,10 +5434,10 @@
         <v>1255</v>
       </c>
       <c r="I30" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J30" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5460,7 +5463,7 @@
         <v>1256</v>
       </c>
       <c r="I31" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -5483,10 +5486,10 @@
         <v>963</v>
       </c>
       <c r="H32" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
       <c r="I32" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -5512,7 +5515,7 @@
         <v>1253</v>
       </c>
       <c r="I33" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -5538,10 +5541,10 @@
         <v>1258</v>
       </c>
       <c r="I34" t="s">
+        <v>1400</v>
+      </c>
+      <c r="J34" t="s">
         <v>1405</v>
-      </c>
-      <c r="J34" t="s">
-        <v>1410</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -5567,10 +5570,10 @@
         <v>1258</v>
       </c>
       <c r="I35" t="s">
+        <v>1400</v>
+      </c>
+      <c r="J35" t="s">
         <v>1405</v>
-      </c>
-      <c r="J35" t="s">
-        <v>1410</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -5596,7 +5599,7 @@
         <v>1259</v>
       </c>
       <c r="I36" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -5619,10 +5622,10 @@
         <v>968</v>
       </c>
       <c r="H37" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="I37" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -5645,10 +5648,10 @@
         <v>969</v>
       </c>
       <c r="H38" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="I38" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -5674,7 +5677,7 @@
         <v>1261</v>
       </c>
       <c r="I39" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -5700,7 +5703,7 @@
         <v>1261</v>
       </c>
       <c r="I40" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -5726,7 +5729,7 @@
         <v>1262</v>
       </c>
       <c r="I41" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -5752,7 +5755,7 @@
         <v>1262</v>
       </c>
       <c r="I42" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -5778,7 +5781,7 @@
         <v>1262</v>
       </c>
       <c r="I43" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -5804,7 +5807,7 @@
         <v>1263</v>
       </c>
       <c r="I44" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -5830,7 +5833,7 @@
         <v>1264</v>
       </c>
       <c r="I45" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -5856,7 +5859,7 @@
         <v>1264</v>
       </c>
       <c r="I46" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -5882,7 +5885,7 @@
         <v>1265</v>
       </c>
       <c r="I47" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -5908,7 +5911,7 @@
         <v>1265</v>
       </c>
       <c r="I48" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -5934,7 +5937,7 @@
         <v>1265</v>
       </c>
       <c r="I49" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -5960,7 +5963,7 @@
         <v>1266</v>
       </c>
       <c r="I50" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -5986,7 +5989,7 @@
         <v>1266</v>
       </c>
       <c r="I51" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -6012,7 +6015,7 @@
         <v>1267</v>
       </c>
       <c r="I52" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -6038,7 +6041,7 @@
         <v>1364</v>
       </c>
       <c r="I53" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -6064,7 +6067,7 @@
         <v>1364</v>
       </c>
       <c r="I54" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -6090,7 +6093,7 @@
         <v>1365</v>
       </c>
       <c r="I55" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -6116,7 +6119,7 @@
         <v>1269</v>
       </c>
       <c r="I56" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -6142,7 +6145,7 @@
         <v>1269</v>
       </c>
       <c r="I57" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -6168,7 +6171,7 @@
         <v>1270</v>
       </c>
       <c r="I58" t="s">
-        <v>1409</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -6194,7 +6197,7 @@
         <v>1253</v>
       </c>
       <c r="I59" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -6220,7 +6223,7 @@
         <v>1254</v>
       </c>
       <c r="I60" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -6246,10 +6249,10 @@
         <v>1255</v>
       </c>
       <c r="I61" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J61" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -6275,10 +6278,10 @@
         <v>1255</v>
       </c>
       <c r="I62" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J62" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -6301,10 +6304,10 @@
         <v>986</v>
       </c>
       <c r="H63" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="I63" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -6330,7 +6333,7 @@
         <v>1256</v>
       </c>
       <c r="I64" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
@@ -6356,10 +6359,10 @@
         <v>1258</v>
       </c>
       <c r="I65" t="s">
+        <v>1400</v>
+      </c>
+      <c r="J65" t="s">
         <v>1405</v>
-      </c>
-      <c r="J65" t="s">
-        <v>1410</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
@@ -6385,7 +6388,7 @@
         <v>1261</v>
       </c>
       <c r="I66" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
@@ -6411,7 +6414,7 @@
         <v>1264</v>
       </c>
       <c r="I67" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
@@ -6437,7 +6440,7 @@
         <v>1265</v>
       </c>
       <c r="I68" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
@@ -6463,7 +6466,7 @@
         <v>1364</v>
       </c>
       <c r="I69" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
@@ -6489,7 +6492,7 @@
         <v>1267</v>
       </c>
       <c r="I70" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
@@ -6515,7 +6518,7 @@
         <v>1364</v>
       </c>
       <c r="I71" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
@@ -6541,7 +6544,7 @@
         <v>1269</v>
       </c>
       <c r="I72" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
@@ -6570,7 +6573,7 @@
         <v>1271</v>
       </c>
       <c r="I73" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
@@ -6593,7 +6596,7 @@
         <v>1271</v>
       </c>
       <c r="I74" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
@@ -6619,7 +6622,7 @@
         <v>1271</v>
       </c>
       <c r="I75" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
@@ -6645,7 +6648,7 @@
         <v>1271</v>
       </c>
       <c r="I76" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
@@ -6671,19 +6674,19 @@
         <v>1271</v>
       </c>
       <c r="I77" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="K77" t="s">
-        <v>1388</v>
+        <v>1414</v>
       </c>
       <c r="L77" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
       <c r="M77" t="s">
         <v>1272</v>
       </c>
       <c r="N77" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
@@ -6712,7 +6715,7 @@
         <v>1272</v>
       </c>
       <c r="I78" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
@@ -6738,7 +6741,7 @@
         <v>1272</v>
       </c>
       <c r="I79" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
@@ -6764,7 +6767,7 @@
         <v>1272</v>
       </c>
       <c r="I80" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -6787,10 +6790,10 @@
         <v>1003</v>
       </c>
       <c r="H81" t="s">
-        <v>1388</v>
+        <v>1414</v>
       </c>
       <c r="I81" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -6813,10 +6816,10 @@
         <v>984</v>
       </c>
       <c r="H82" t="s">
-        <v>1388</v>
+        <v>1414</v>
       </c>
       <c r="I82" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
@@ -6839,10 +6842,10 @@
         <v>1004</v>
       </c>
       <c r="H83" t="s">
-        <v>1390</v>
+        <v>1416</v>
       </c>
       <c r="I83" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
@@ -6865,10 +6868,10 @@
         <v>1005</v>
       </c>
       <c r="H84" t="s">
-        <v>1390</v>
+        <v>1416</v>
       </c>
       <c r="I84" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
@@ -6891,10 +6894,10 @@
         <v>1006</v>
       </c>
       <c r="H85" t="s">
-        <v>1390</v>
+        <v>1416</v>
       </c>
       <c r="I85" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -6920,7 +6923,7 @@
         <v>1273</v>
       </c>
       <c r="I86" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
@@ -6946,7 +6949,7 @@
         <v>1273</v>
       </c>
       <c r="I87" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -6969,10 +6972,10 @@
         <v>1009</v>
       </c>
       <c r="H88" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="I88" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -6995,10 +6998,10 @@
         <v>1010</v>
       </c>
       <c r="H89" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="I89" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
@@ -7021,13 +7024,13 @@
         <v>1011</v>
       </c>
       <c r="H90" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I90" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J90" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -7050,13 +7053,13 @@
         <v>1012</v>
       </c>
       <c r="H91" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I91" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J91" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -7079,13 +7082,13 @@
         <v>1013</v>
       </c>
       <c r="H92" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I92" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J92" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -7108,13 +7111,13 @@
         <v>1014</v>
       </c>
       <c r="H93" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I93" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J93" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -7137,13 +7140,13 @@
         <v>1015</v>
       </c>
       <c r="H94" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I94" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J94" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
@@ -7169,7 +7172,7 @@
         <v>1275</v>
       </c>
       <c r="I95" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -7195,7 +7198,7 @@
         <v>1276</v>
       </c>
       <c r="I96" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -7221,7 +7224,7 @@
         <v>1276</v>
       </c>
       <c r="I97" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -7247,7 +7250,7 @@
         <v>1276</v>
       </c>
       <c r="I98" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -7273,7 +7276,7 @@
         <v>1276</v>
       </c>
       <c r="I99" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -7299,7 +7302,7 @@
         <v>1276</v>
       </c>
       <c r="I100" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -7325,7 +7328,7 @@
         <v>1366</v>
       </c>
       <c r="I101" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
@@ -7351,7 +7354,7 @@
         <v>1366</v>
       </c>
       <c r="I102" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -7377,7 +7380,7 @@
         <v>1367</v>
       </c>
       <c r="I103" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -7403,7 +7406,7 @@
         <v>1368</v>
       </c>
       <c r="I104" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -7429,7 +7432,7 @@
         <v>1368</v>
       </c>
       <c r="I105" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -7455,7 +7458,7 @@
         <v>1369</v>
       </c>
       <c r="I106" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
@@ -7481,7 +7484,7 @@
         <v>1369</v>
       </c>
       <c r="I107" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
@@ -7504,10 +7507,10 @@
         <v>1028</v>
       </c>
       <c r="H108" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="I108" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
@@ -7530,10 +7533,10 @@
         <v>1029</v>
       </c>
       <c r="H109" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="I109" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -7559,7 +7562,7 @@
         <v>1277</v>
       </c>
       <c r="I110" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -7585,7 +7588,7 @@
         <v>1277</v>
       </c>
       <c r="I111" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -7611,7 +7614,7 @@
         <v>1278</v>
       </c>
       <c r="I112" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
@@ -7637,7 +7640,7 @@
         <v>1278</v>
       </c>
       <c r="I113" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -7663,7 +7666,7 @@
         <v>1278</v>
       </c>
       <c r="I114" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
@@ -7689,7 +7692,7 @@
         <v>1279</v>
       </c>
       <c r="I115" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -7715,7 +7718,7 @@
         <v>1279</v>
       </c>
       <c r="I116" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -7741,7 +7744,7 @@
         <v>1279</v>
       </c>
       <c r="I117" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -7767,7 +7770,7 @@
         <v>1279</v>
       </c>
       <c r="I118" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -7790,10 +7793,10 @@
         <v>1035</v>
       </c>
       <c r="H119" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I119" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -7816,10 +7819,10 @@
         <v>944</v>
       </c>
       <c r="H120" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I120" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -7845,7 +7848,7 @@
         <v>1370</v>
       </c>
       <c r="I121" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -7871,7 +7874,7 @@
         <v>1370</v>
       </c>
       <c r="I122" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -7897,7 +7900,7 @@
         <v>1281</v>
       </c>
       <c r="I123" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
@@ -7923,7 +7926,7 @@
         <v>1281</v>
       </c>
       <c r="I124" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
@@ -7949,7 +7952,7 @@
         <v>1282</v>
       </c>
       <c r="I125" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -7975,7 +7978,7 @@
         <v>1282</v>
       </c>
       <c r="I126" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -8001,7 +8004,7 @@
         <v>1283</v>
       </c>
       <c r="I127" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
@@ -8027,7 +8030,7 @@
         <v>1284</v>
       </c>
       <c r="I128" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
@@ -8053,7 +8056,7 @@
         <v>1284</v>
       </c>
       <c r="I129" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -8079,7 +8082,7 @@
         <v>1285</v>
       </c>
       <c r="I130" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -8102,10 +8105,10 @@
         <v>951</v>
       </c>
       <c r="H131" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="I131" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -8131,7 +8134,7 @@
         <v>1286</v>
       </c>
       <c r="I132" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -8157,7 +8160,7 @@
         <v>1287</v>
       </c>
       <c r="I133" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
@@ -8183,7 +8186,7 @@
         <v>1287</v>
       </c>
       <c r="I134" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
@@ -8209,7 +8212,7 @@
         <v>1288</v>
       </c>
       <c r="I135" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
@@ -8235,7 +8238,7 @@
         <v>1288</v>
       </c>
       <c r="I136" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
@@ -8261,7 +8264,7 @@
         <v>1289</v>
       </c>
       <c r="I137" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -8287,7 +8290,7 @@
         <v>1289</v>
       </c>
       <c r="I138" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
@@ -8313,7 +8316,7 @@
         <v>1290</v>
       </c>
       <c r="I139" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -8336,10 +8339,10 @@
         <v>1052</v>
       </c>
       <c r="H140" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
       <c r="I140" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
@@ -8361,11 +8364,11 @@
       <c r="G141" t="s">
         <v>1053</v>
       </c>
-      <c r="H141" t="s">
-        <v>1396</v>
+      <c r="H141" s="1" t="s">
+        <v>1415</v>
       </c>
       <c r="I141" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
@@ -8388,10 +8391,10 @@
         <v>1054</v>
       </c>
       <c r="H142" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="I142" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
@@ -8414,10 +8417,10 @@
         <v>1055</v>
       </c>
       <c r="H143" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="I143" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
@@ -8443,7 +8446,7 @@
         <v>1291</v>
       </c>
       <c r="I144" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
@@ -8469,7 +8472,7 @@
         <v>1291</v>
       </c>
       <c r="I145" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
@@ -8495,7 +8498,7 @@
         <v>1291</v>
       </c>
       <c r="I146" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
@@ -8521,7 +8524,7 @@
         <v>1291</v>
       </c>
       <c r="I147" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
@@ -8547,7 +8550,7 @@
         <v>1291</v>
       </c>
       <c r="I148" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
@@ -8573,7 +8576,7 @@
         <v>1292</v>
       </c>
       <c r="I149" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
@@ -8599,7 +8602,7 @@
         <v>1268</v>
       </c>
       <c r="I150" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
@@ -8625,7 +8628,7 @@
         <v>1268</v>
       </c>
       <c r="I151" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
@@ -8651,7 +8654,7 @@
         <v>1268</v>
       </c>
       <c r="I152" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -8674,10 +8677,10 @@
         <v>1063</v>
       </c>
       <c r="H153" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="I153" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -8700,10 +8703,10 @@
         <v>1064</v>
       </c>
       <c r="H154" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="I154" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
@@ -8726,10 +8729,10 @@
         <v>1051</v>
       </c>
       <c r="H155" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="I155" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
@@ -8755,7 +8758,7 @@
         <v>1371</v>
       </c>
       <c r="I156" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -8781,7 +8784,7 @@
         <v>1371</v>
       </c>
       <c r="I157" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
@@ -8807,7 +8810,7 @@
         <v>1371</v>
       </c>
       <c r="I158" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
@@ -8833,7 +8836,7 @@
         <v>1371</v>
       </c>
       <c r="I159" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
@@ -8856,10 +8859,10 @@
         <v>1069</v>
       </c>
       <c r="H160" t="s">
-        <v>1372</v>
+        <v>1418</v>
       </c>
       <c r="I160" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
@@ -8882,10 +8885,10 @@
         <v>1070</v>
       </c>
       <c r="H161" t="s">
-        <v>1372</v>
+        <v>1418</v>
       </c>
       <c r="I161" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
@@ -8908,10 +8911,10 @@
         <v>1030</v>
       </c>
       <c r="H162" t="s">
-        <v>1372</v>
+        <v>1418</v>
       </c>
       <c r="I162" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
@@ -8934,10 +8937,10 @@
         <v>1071</v>
       </c>
       <c r="H163" t="s">
-        <v>1372</v>
+        <v>1418</v>
       </c>
       <c r="I163" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
@@ -8963,7 +8966,7 @@
         <v>1293</v>
       </c>
       <c r="I164" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
@@ -8989,7 +8992,7 @@
         <v>1293</v>
       </c>
       <c r="I165" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
@@ -9015,7 +9018,7 @@
         <v>1293</v>
       </c>
       <c r="I166" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
@@ -9041,7 +9044,7 @@
         <v>1293</v>
       </c>
       <c r="I167" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
@@ -9067,7 +9070,7 @@
         <v>1293</v>
       </c>
       <c r="I168" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
@@ -9090,10 +9093,10 @@
         <v>1076</v>
       </c>
       <c r="H169" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="I169" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
@@ -9116,10 +9119,10 @@
         <v>1077</v>
       </c>
       <c r="H170" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="I170" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -9142,10 +9145,10 @@
         <v>1078</v>
       </c>
       <c r="H171" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="I171" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
@@ -9171,7 +9174,7 @@
         <v>1294</v>
       </c>
       <c r="I172" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
@@ -9194,10 +9197,10 @@
         <v>1036</v>
       </c>
       <c r="H173" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="I173" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
@@ -9223,7 +9226,7 @@
         <v>1295</v>
       </c>
       <c r="I174" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
@@ -9249,7 +9252,7 @@
         <v>1295</v>
       </c>
       <c r="I175" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
@@ -9272,10 +9275,10 @@
         <v>1081</v>
       </c>
       <c r="H176" t="s">
-        <v>1400</v>
+        <v>1417</v>
       </c>
       <c r="I176" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.3">
@@ -9298,10 +9301,10 @@
         <v>1082</v>
       </c>
       <c r="H177" t="s">
-        <v>1400</v>
+        <v>1417</v>
       </c>
       <c r="I177" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.3">
@@ -9327,43 +9330,43 @@
         <v>1367</v>
       </c>
       <c r="I178" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="K178" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="L178" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
       <c r="M178" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="N178" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
       <c r="O178" t="s">
         <v>1279</v>
       </c>
       <c r="P178" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
       <c r="Q178" t="s">
         <v>1281</v>
       </c>
       <c r="R178" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
       <c r="S178" t="s">
         <v>1287</v>
       </c>
       <c r="T178" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
       <c r="U178" t="s">
-        <v>1411</v>
+        <v>1406</v>
       </c>
       <c r="V178" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.3">
@@ -9389,7 +9392,7 @@
         <v>1296</v>
       </c>
       <c r="I179" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.3">
@@ -9415,7 +9418,7 @@
         <v>1296</v>
       </c>
       <c r="I180" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.3">
@@ -9441,7 +9444,7 @@
         <v>1296</v>
       </c>
       <c r="I181" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.3">
@@ -9467,7 +9470,7 @@
         <v>1296</v>
       </c>
       <c r="I182" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.3">
@@ -9493,7 +9496,7 @@
         <v>1296</v>
       </c>
       <c r="I183" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.3">
@@ -9516,10 +9519,10 @@
         <v>1088</v>
       </c>
       <c r="H184" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="I184" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.3">
@@ -9542,10 +9545,10 @@
         <v>1089</v>
       </c>
       <c r="H185" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="I185" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.3">
@@ -9568,10 +9571,10 @@
         <v>1090</v>
       </c>
       <c r="H186" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="I186" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.3">
@@ -9594,10 +9597,10 @@
         <v>1091</v>
       </c>
       <c r="H187" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="I187" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.3">
@@ -9620,10 +9623,10 @@
         <v>981</v>
       </c>
       <c r="H188" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="I188" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="189" spans="1:22" x14ac:dyDescent="0.3">
@@ -9649,7 +9652,7 @@
         <v>1297</v>
       </c>
       <c r="I189" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="190" spans="1:22" x14ac:dyDescent="0.3">
@@ -9675,7 +9678,7 @@
         <v>1297</v>
       </c>
       <c r="I190" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="191" spans="1:22" x14ac:dyDescent="0.3">
@@ -9701,7 +9704,7 @@
         <v>1297</v>
       </c>
       <c r="I191" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.3">
@@ -9727,7 +9730,7 @@
         <v>1297</v>
       </c>
       <c r="I192" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.3">
@@ -9750,10 +9753,10 @@
         <v>1096</v>
       </c>
       <c r="H193" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="I193" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.3">
@@ -9776,10 +9779,10 @@
         <v>1097</v>
       </c>
       <c r="H194" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="I194" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.3">
@@ -9802,10 +9805,10 @@
         <v>1098</v>
       </c>
       <c r="H195" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="I195" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.3">
@@ -9831,7 +9834,7 @@
         <v>1299</v>
       </c>
       <c r="I196" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.3">
@@ -9857,10 +9860,10 @@
         <v>1300</v>
       </c>
       <c r="I197" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J197" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.3">
@@ -9886,10 +9889,10 @@
         <v>1300</v>
       </c>
       <c r="I198" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J198" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.3">
@@ -9915,10 +9918,10 @@
         <v>1300</v>
       </c>
       <c r="I199" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J199" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.3">
@@ -9944,10 +9947,10 @@
         <v>1300</v>
       </c>
       <c r="I200" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J200" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.3">
@@ -9973,10 +9976,10 @@
         <v>1300</v>
       </c>
       <c r="I201" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J201" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.3">
@@ -10002,7 +10005,7 @@
         <v>1299</v>
       </c>
       <c r="I202" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.3">
@@ -10028,7 +10031,7 @@
         <v>1299</v>
       </c>
       <c r="I203" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.3">
@@ -10054,7 +10057,7 @@
         <v>1301</v>
       </c>
       <c r="I204" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.3">
@@ -10080,7 +10083,7 @@
         <v>1301</v>
       </c>
       <c r="I205" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.3">
@@ -10106,7 +10109,7 @@
         <v>1301</v>
       </c>
       <c r="I206" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.3">
@@ -10132,7 +10135,7 @@
         <v>1301</v>
       </c>
       <c r="I207" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.3">
@@ -10158,7 +10161,7 @@
         <v>1301</v>
       </c>
       <c r="I208" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
@@ -10184,7 +10187,7 @@
         <v>1260</v>
       </c>
       <c r="I209" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
@@ -10210,7 +10213,7 @@
         <v>1302</v>
       </c>
       <c r="I210" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
@@ -10236,7 +10239,7 @@
         <v>1302</v>
       </c>
       <c r="I211" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
@@ -10262,7 +10265,7 @@
         <v>1302</v>
       </c>
       <c r="I212" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
@@ -10288,7 +10291,7 @@
         <v>1303</v>
       </c>
       <c r="I213" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
@@ -10314,7 +10317,7 @@
         <v>1303</v>
       </c>
       <c r="I214" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
@@ -10340,7 +10343,7 @@
         <v>1303</v>
       </c>
       <c r="I215" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
@@ -10366,7 +10369,7 @@
         <v>1303</v>
       </c>
       <c r="I216" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
@@ -10392,7 +10395,7 @@
         <v>1303</v>
       </c>
       <c r="I217" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
@@ -10415,10 +10418,10 @@
         <v>1115</v>
       </c>
       <c r="H218" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I218" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
@@ -10441,10 +10444,10 @@
         <v>1090</v>
       </c>
       <c r="H219" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I219" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
@@ -10467,10 +10470,10 @@
         <v>1035</v>
       </c>
       <c r="H220" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I220" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
@@ -10493,10 +10496,10 @@
         <v>1046</v>
       </c>
       <c r="H221" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I221" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
@@ -10519,10 +10522,10 @@
         <v>1051</v>
       </c>
       <c r="H222" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I222" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
@@ -10548,7 +10551,7 @@
         <v>1304</v>
       </c>
       <c r="I223" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
@@ -10574,7 +10577,7 @@
         <v>1304</v>
       </c>
       <c r="I224" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.3">
@@ -10600,7 +10603,7 @@
         <v>1304</v>
       </c>
       <c r="I225" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.3">
@@ -10626,7 +10629,7 @@
         <v>1304</v>
       </c>
       <c r="I226" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.3">
@@ -10652,7 +10655,7 @@
         <v>1304</v>
       </c>
       <c r="I227" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.3">
@@ -10678,7 +10681,7 @@
         <v>1305</v>
       </c>
       <c r="I228" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.3">
@@ -10704,7 +10707,7 @@
         <v>1305</v>
       </c>
       <c r="I229" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.3">
@@ -10730,7 +10733,7 @@
         <v>1305</v>
       </c>
       <c r="I230" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.3">
@@ -10756,7 +10759,7 @@
         <v>1306</v>
       </c>
       <c r="I231" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.3">
@@ -10782,10 +10785,10 @@
         <v>1307</v>
       </c>
       <c r="I232" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
       <c r="J232" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.3">
@@ -10811,7 +10814,7 @@
         <v>1306</v>
       </c>
       <c r="I233" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.3">
@@ -10837,10 +10840,10 @@
         <v>1307</v>
       </c>
       <c r="I234" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
       <c r="J234" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.3">
@@ -10866,7 +10869,7 @@
         <v>1308</v>
       </c>
       <c r="I235" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.3">
@@ -10889,10 +10892,10 @@
         <v>1124</v>
       </c>
       <c r="H236" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="I236" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.3">
@@ -10918,7 +10921,7 @@
         <v>1306</v>
       </c>
       <c r="I237" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.3">
@@ -10944,7 +10947,7 @@
         <v>1254</v>
       </c>
       <c r="I238" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.3">
@@ -10970,7 +10973,7 @@
         <v>1254</v>
       </c>
       <c r="I239" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.3">
@@ -10996,7 +10999,7 @@
         <v>1254</v>
       </c>
       <c r="I240" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.3">
@@ -11022,7 +11025,7 @@
         <v>1309</v>
       </c>
       <c r="I241" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.3">
@@ -11045,10 +11048,10 @@
         <v>1129</v>
       </c>
       <c r="H242" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="I242" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.3">
@@ -11074,10 +11077,10 @@
         <v>1307</v>
       </c>
       <c r="I243" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
       <c r="J243" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.3">
@@ -11100,10 +11103,10 @@
         <v>1073</v>
       </c>
       <c r="H244" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="I244" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.3">
@@ -11126,10 +11129,10 @@
         <v>1131</v>
       </c>
       <c r="H245" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="I245" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.3">
@@ -11155,7 +11158,7 @@
         <v>1309</v>
       </c>
       <c r="I246" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.3">
@@ -11178,10 +11181,10 @@
         <v>985</v>
       </c>
       <c r="H247" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="I247" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.3">
@@ -11207,7 +11210,7 @@
         <v>1306</v>
       </c>
       <c r="I248" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.3">
@@ -11233,7 +11236,7 @@
         <v>1306</v>
       </c>
       <c r="I249" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.3">
@@ -11256,10 +11259,10 @@
         <v>991</v>
       </c>
       <c r="H250" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="I250" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.3">
@@ -11285,7 +11288,7 @@
         <v>1306</v>
       </c>
       <c r="I251" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.3">
@@ -11308,10 +11311,10 @@
         <v>1135</v>
       </c>
       <c r="H252" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="I252" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.3">
@@ -11337,7 +11340,7 @@
         <v>1310</v>
       </c>
       <c r="I253" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.3">
@@ -11363,7 +11366,7 @@
         <v>1311</v>
       </c>
       <c r="I254" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.3">
@@ -11389,7 +11392,7 @@
         <v>1311</v>
       </c>
       <c r="I255" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.3">
@@ -11415,7 +11418,7 @@
         <v>1311</v>
       </c>
       <c r="I256" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.3">
@@ -11441,7 +11444,7 @@
         <v>1311</v>
       </c>
       <c r="I257" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
@@ -11467,7 +11470,7 @@
         <v>1312</v>
       </c>
       <c r="I258" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.3">
@@ -11493,7 +11496,7 @@
         <v>1270</v>
       </c>
       <c r="I259" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.3">
@@ -11519,7 +11522,7 @@
         <v>1270</v>
       </c>
       <c r="I260" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.3">
@@ -11545,7 +11548,7 @@
         <v>1313</v>
       </c>
       <c r="I261" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.3">
@@ -11571,7 +11574,7 @@
         <v>1270</v>
       </c>
       <c r="I262" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.3">
@@ -11597,7 +11600,7 @@
         <v>1248</v>
       </c>
       <c r="I263" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.3">
@@ -11623,7 +11626,7 @@
         <v>1248</v>
       </c>
       <c r="I264" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.3">
@@ -11649,7 +11652,7 @@
         <v>1274</v>
       </c>
       <c r="I265" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.3">
@@ -11675,7 +11678,7 @@
         <v>1274</v>
       </c>
       <c r="I266" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.3">
@@ -11701,7 +11704,7 @@
         <v>1274</v>
       </c>
       <c r="I267" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.3">
@@ -11727,7 +11730,7 @@
         <v>1313</v>
       </c>
       <c r="I268" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.3">
@@ -11753,7 +11756,7 @@
         <v>1314</v>
       </c>
       <c r="I269" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.3">
@@ -11779,7 +11782,7 @@
         <v>1313</v>
       </c>
       <c r="I270" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.3">
@@ -11805,7 +11808,7 @@
         <v>1314</v>
       </c>
       <c r="I271" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.3">
@@ -11828,10 +11831,10 @@
         <v>968</v>
       </c>
       <c r="H272" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="I272" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.3">
@@ -11854,10 +11857,10 @@
         <v>1146</v>
       </c>
       <c r="H273" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="I273" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
@@ -11883,7 +11886,7 @@
         <v>1316</v>
       </c>
       <c r="I274" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
@@ -11909,7 +11912,7 @@
         <v>1314</v>
       </c>
       <c r="I275" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
@@ -11935,7 +11938,7 @@
         <v>1314</v>
       </c>
       <c r="I276" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
@@ -11961,7 +11964,7 @@
         <v>1314</v>
       </c>
       <c r="I277" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -11987,7 +11990,7 @@
         <v>1313</v>
       </c>
       <c r="I278" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
@@ -12013,7 +12016,7 @@
         <v>1313</v>
       </c>
       <c r="I279" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
@@ -12039,7 +12042,7 @@
         <v>1314</v>
       </c>
       <c r="I280" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
@@ -12062,10 +12065,10 @@
         <v>1149</v>
       </c>
       <c r="H281" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="I281" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
@@ -12091,7 +12094,7 @@
         <v>1317</v>
       </c>
       <c r="I282" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
@@ -12117,7 +12120,7 @@
         <v>1313</v>
       </c>
       <c r="I283" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
@@ -12143,7 +12146,7 @@
         <v>1317</v>
       </c>
       <c r="I284" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
@@ -12169,7 +12172,7 @@
         <v>1318</v>
       </c>
       <c r="I285" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
@@ -12198,7 +12201,7 @@
         <v>1318</v>
       </c>
       <c r="I286" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -12224,7 +12227,7 @@
         <v>1318</v>
       </c>
       <c r="I287" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -12247,10 +12250,10 @@
         <v>1035</v>
       </c>
       <c r="H288" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="I288" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.3">
@@ -12273,10 +12276,10 @@
         <v>945</v>
       </c>
       <c r="H289" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="I289" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
@@ -12299,10 +12302,10 @@
         <v>967</v>
       </c>
       <c r="H290" t="s">
-        <v>1414</v>
+        <v>1409</v>
       </c>
       <c r="I290" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
@@ -12328,7 +12331,7 @@
         <v>1318</v>
       </c>
       <c r="I291" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
@@ -12354,7 +12357,7 @@
         <v>1318</v>
       </c>
       <c r="I292" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
@@ -12377,10 +12380,10 @@
         <v>944</v>
       </c>
       <c r="H293" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="I293" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
@@ -12403,10 +12406,10 @@
         <v>1154</v>
       </c>
       <c r="H294" t="s">
-        <v>1414</v>
+        <v>1409</v>
       </c>
       <c r="I294" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -12432,7 +12435,7 @@
         <v>1318</v>
       </c>
       <c r="I295" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
@@ -12455,10 +12458,10 @@
         <v>1134</v>
       </c>
       <c r="H296" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="I296" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
@@ -12481,10 +12484,10 @@
         <v>1155</v>
       </c>
       <c r="H297" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="I297" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
@@ -12507,10 +12510,10 @@
         <v>1156</v>
       </c>
       <c r="H298" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="I298" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
@@ -12533,10 +12536,10 @@
         <v>1157</v>
       </c>
       <c r="H299" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="I299" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
@@ -12559,10 +12562,10 @@
         <v>943</v>
       </c>
       <c r="H300" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="I300" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
@@ -12585,10 +12588,10 @@
         <v>1064</v>
       </c>
       <c r="H301" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="I301" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -12614,7 +12617,7 @@
         <v>1319</v>
       </c>
       <c r="I302" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -12640,7 +12643,7 @@
         <v>1319</v>
       </c>
       <c r="I303" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
@@ -12663,10 +12666,10 @@
         <v>1159</v>
       </c>
       <c r="H304" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="I304" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.3">
@@ -12689,10 +12692,10 @@
         <v>1160</v>
       </c>
       <c r="H305" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="I305" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
@@ -12718,7 +12721,7 @@
         <v>1319</v>
       </c>
       <c r="I306" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.3">
@@ -12744,7 +12747,7 @@
         <v>1320</v>
       </c>
       <c r="I307" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.3">
@@ -12767,10 +12770,10 @@
         <v>1085</v>
       </c>
       <c r="H308" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="I308" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
@@ -12793,10 +12796,10 @@
         <v>1163</v>
       </c>
       <c r="H309" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="I309" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
@@ -12822,7 +12825,7 @@
         <v>1320</v>
       </c>
       <c r="I310" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
@@ -12848,7 +12851,7 @@
         <v>1320</v>
       </c>
       <c r="I311" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
@@ -12874,7 +12877,7 @@
         <v>1320</v>
       </c>
       <c r="I312" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
@@ -12900,7 +12903,7 @@
         <v>1319</v>
       </c>
       <c r="I313" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.3">
@@ -12923,10 +12926,10 @@
         <v>986</v>
       </c>
       <c r="H314" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="I314" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -12949,10 +12952,10 @@
         <v>968</v>
       </c>
       <c r="H315" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="I315" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.3">
@@ -12978,7 +12981,7 @@
         <v>1316</v>
       </c>
       <c r="I316" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -13004,7 +13007,7 @@
         <v>1316</v>
       </c>
       <c r="I317" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -13030,7 +13033,7 @@
         <v>1316</v>
       </c>
       <c r="I318" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -13056,7 +13059,7 @@
         <v>1249</v>
       </c>
       <c r="I319" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -13079,10 +13082,10 @@
         <v>1168</v>
       </c>
       <c r="H320" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="I320" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
@@ -13108,7 +13111,7 @@
         <v>1321</v>
       </c>
       <c r="I321" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
@@ -13134,7 +13137,7 @@
         <v>1321</v>
       </c>
       <c r="I322" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -13160,7 +13163,7 @@
         <v>1322</v>
       </c>
       <c r="I323" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
@@ -13186,7 +13189,7 @@
         <v>1323</v>
       </c>
       <c r="I324" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
@@ -13212,7 +13215,7 @@
         <v>1324</v>
       </c>
       <c r="I325" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -13238,7 +13241,7 @@
         <v>1322</v>
       </c>
       <c r="I326" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
@@ -13264,7 +13267,7 @@
         <v>1316</v>
       </c>
       <c r="I327" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
@@ -13287,10 +13290,10 @@
         <v>1172</v>
       </c>
       <c r="H328" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="I328" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -13316,7 +13319,7 @@
         <v>1321</v>
       </c>
       <c r="I329" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -13339,10 +13342,10 @@
         <v>1140</v>
       </c>
       <c r="H330" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="I330" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -13365,10 +13368,10 @@
         <v>1173</v>
       </c>
       <c r="H331" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="I331" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
@@ -13394,7 +13397,7 @@
         <v>1323</v>
       </c>
       <c r="I332" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -13420,7 +13423,7 @@
         <v>1325</v>
       </c>
       <c r="I333" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -13446,7 +13449,7 @@
         <v>1325</v>
       </c>
       <c r="I334" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -13472,7 +13475,7 @@
         <v>1326</v>
       </c>
       <c r="I335" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -13498,7 +13501,7 @@
         <v>1327</v>
       </c>
       <c r="I336" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.3">
@@ -13524,7 +13527,7 @@
         <v>1257</v>
       </c>
       <c r="I337" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -13550,7 +13553,7 @@
         <v>1257</v>
       </c>
       <c r="I338" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
@@ -13576,7 +13579,7 @@
         <v>1327</v>
       </c>
       <c r="I339" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.3">
@@ -13602,7 +13605,7 @@
         <v>1325</v>
       </c>
       <c r="I340" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
@@ -13628,7 +13631,7 @@
         <v>1328</v>
       </c>
       <c r="I341" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.3">
@@ -13654,7 +13657,7 @@
         <v>1328</v>
       </c>
       <c r="I342" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.3">
@@ -13680,7 +13683,7 @@
         <v>1328</v>
       </c>
       <c r="I343" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
@@ -13706,7 +13709,7 @@
         <v>1328</v>
       </c>
       <c r="I344" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
@@ -13732,7 +13735,7 @@
         <v>1329</v>
       </c>
       <c r="I345" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.3">
@@ -13758,7 +13761,7 @@
         <v>1329</v>
       </c>
       <c r="I346" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
@@ -13784,7 +13787,7 @@
         <v>1329</v>
       </c>
       <c r="I347" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.3">
@@ -13810,7 +13813,7 @@
         <v>1329</v>
       </c>
       <c r="I348" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.3">
@@ -13836,7 +13839,7 @@
         <v>1298</v>
       </c>
       <c r="I349" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
@@ -13862,7 +13865,7 @@
         <v>1270</v>
       </c>
       <c r="I350" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
@@ -13885,10 +13888,10 @@
         <v>1179</v>
       </c>
       <c r="H351" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="I351" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
@@ -13911,10 +13914,10 @@
         <v>1180</v>
       </c>
       <c r="H352" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="I352" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.3">
@@ -13940,7 +13943,7 @@
         <v>1330</v>
       </c>
       <c r="I353" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
@@ -13966,7 +13969,7 @@
         <v>1330</v>
       </c>
       <c r="I354" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.3">
@@ -13992,7 +13995,7 @@
         <v>1331</v>
       </c>
       <c r="I355" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.3">
@@ -14018,7 +14021,7 @@
         <v>1331</v>
       </c>
       <c r="I356" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -14044,7 +14047,7 @@
         <v>1330</v>
       </c>
       <c r="I357" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="358" spans="1:9" x14ac:dyDescent="0.3">
@@ -14067,10 +14070,10 @@
         <v>950</v>
       </c>
       <c r="H358" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="I358" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
@@ -14099,7 +14102,7 @@
         <v>1280</v>
       </c>
       <c r="I359" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -14128,7 +14131,7 @@
         <v>1280</v>
       </c>
       <c r="I360" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.3">
@@ -14157,7 +14160,7 @@
         <v>1280</v>
       </c>
       <c r="I361" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -14180,10 +14183,10 @@
         <v>939</v>
       </c>
       <c r="H362" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I362" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
@@ -14206,10 +14209,10 @@
         <v>1186</v>
       </c>
       <c r="H363" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I363" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.3">
@@ -14232,10 +14235,10 @@
         <v>1187</v>
       </c>
       <c r="H364" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I364" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.3">
@@ -14258,10 +14261,10 @@
         <v>1188</v>
       </c>
       <c r="H365" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I365" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.3">
@@ -14284,10 +14287,10 @@
         <v>1189</v>
       </c>
       <c r="H366" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I366" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.3">
@@ -14310,10 +14313,10 @@
         <v>1021</v>
       </c>
       <c r="H367" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I367" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.3">
@@ -14339,7 +14342,7 @@
         <v>1332</v>
       </c>
       <c r="I368" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.3">
@@ -14365,7 +14368,7 @@
         <v>1332</v>
       </c>
       <c r="I369" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.3">
@@ -14391,7 +14394,7 @@
         <v>1333</v>
       </c>
       <c r="I370" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="371" spans="1:12" x14ac:dyDescent="0.3">
@@ -14417,7 +14420,7 @@
         <v>1333</v>
       </c>
       <c r="I371" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="372" spans="1:12" x14ac:dyDescent="0.3">
@@ -14443,7 +14446,7 @@
         <v>1334</v>
       </c>
       <c r="I372" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="373" spans="1:12" x14ac:dyDescent="0.3">
@@ -14469,7 +14472,7 @@
         <v>1335</v>
       </c>
       <c r="I373" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.3">
@@ -14495,7 +14498,7 @@
         <v>1335</v>
       </c>
       <c r="I374" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="375" spans="1:12" x14ac:dyDescent="0.3">
@@ -14521,7 +14524,7 @@
         <v>1336</v>
       </c>
       <c r="I375" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="376" spans="1:12" x14ac:dyDescent="0.3">
@@ -14547,7 +14550,7 @@
         <v>1332</v>
       </c>
       <c r="I376" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="377" spans="1:12" x14ac:dyDescent="0.3">
@@ -14573,7 +14576,7 @@
         <v>1332</v>
       </c>
       <c r="I377" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="K377" t="s">
         <v>1332</v>
@@ -14599,16 +14602,16 @@
         <v>1194</v>
       </c>
       <c r="H378" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="I378" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="K378" t="s">
         <v>1332</v>
       </c>
       <c r="L378" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.3">
@@ -14637,7 +14640,7 @@
         <v>1337</v>
       </c>
       <c r="I379" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.3">
@@ -14663,7 +14666,7 @@
         <v>1337</v>
       </c>
       <c r="I380" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="381" spans="1:12" x14ac:dyDescent="0.3">
@@ -14689,7 +14692,7 @@
         <v>1337</v>
       </c>
       <c r="I381" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.3">
@@ -14715,7 +14718,7 @@
         <v>1337</v>
       </c>
       <c r="I382" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.3">
@@ -14741,7 +14744,7 @@
         <v>1337</v>
       </c>
       <c r="I383" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.3">
@@ -14767,13 +14770,13 @@
         <v>1337</v>
       </c>
       <c r="I384" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="K384" t="s">
         <v>1341</v>
       </c>
       <c r="L384" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="385" spans="1:12" x14ac:dyDescent="0.3">
@@ -14799,13 +14802,13 @@
         <v>1337</v>
       </c>
       <c r="I385" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="K385" t="s">
         <v>1315</v>
       </c>
       <c r="L385" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.3">
@@ -14831,7 +14834,7 @@
         <v>1338</v>
       </c>
       <c r="I386" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.3">
@@ -14857,7 +14860,7 @@
         <v>1338</v>
       </c>
       <c r="I387" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.3">
@@ -14883,7 +14886,7 @@
         <v>1338</v>
       </c>
       <c r="I388" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.3">
@@ -14909,7 +14912,7 @@
         <v>1338</v>
       </c>
       <c r="I389" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.3">
@@ -14935,7 +14938,7 @@
         <v>1338</v>
       </c>
       <c r="I390" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.3">
@@ -14961,7 +14964,7 @@
         <v>1338</v>
       </c>
       <c r="I391" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.3">
@@ -14987,7 +14990,7 @@
         <v>1338</v>
       </c>
       <c r="I392" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.3">
@@ -15013,7 +15016,7 @@
         <v>1339</v>
       </c>
       <c r="I393" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.3">
@@ -15039,7 +15042,7 @@
         <v>1340</v>
       </c>
       <c r="I394" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.3">
@@ -15065,7 +15068,7 @@
         <v>1341</v>
       </c>
       <c r="I395" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.3">
@@ -15091,7 +15094,7 @@
         <v>1315</v>
       </c>
       <c r="I396" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.3">
@@ -15117,7 +15120,7 @@
         <v>1315</v>
       </c>
       <c r="I397" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.3">
@@ -15143,7 +15146,7 @@
         <v>1342</v>
       </c>
       <c r="I398" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.3">
@@ -15172,7 +15175,7 @@
         <v>1343</v>
       </c>
       <c r="I399" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.3">
@@ -15201,7 +15204,7 @@
         <v>1343</v>
       </c>
       <c r="I400" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.3">
@@ -15230,7 +15233,7 @@
         <v>1343</v>
       </c>
       <c r="I401" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.3">
@@ -15259,7 +15262,7 @@
         <v>1343</v>
       </c>
       <c r="I402" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.3">
@@ -15288,7 +15291,7 @@
         <v>1343</v>
       </c>
       <c r="I403" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="404" spans="1:9" x14ac:dyDescent="0.3">
@@ -15317,7 +15320,7 @@
         <v>1343</v>
       </c>
       <c r="I404" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.3">
@@ -15346,7 +15349,7 @@
         <v>1343</v>
       </c>
       <c r="I405" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.3">
@@ -15375,7 +15378,7 @@
         <v>1343</v>
       </c>
       <c r="I406" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="407" spans="1:9" x14ac:dyDescent="0.3">
@@ -15404,7 +15407,7 @@
         <v>1343</v>
       </c>
       <c r="I407" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.3">
@@ -15430,7 +15433,7 @@
         <v>1343</v>
       </c>
       <c r="I408" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="409" spans="1:9" x14ac:dyDescent="0.3">
@@ -15459,7 +15462,7 @@
         <v>1344</v>
       </c>
       <c r="I409" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="410" spans="1:9" x14ac:dyDescent="0.3">
@@ -15488,7 +15491,7 @@
         <v>1344</v>
       </c>
       <c r="I410" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.3">
@@ -15517,7 +15520,7 @@
         <v>1344</v>
       </c>
       <c r="I411" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="412" spans="1:9" x14ac:dyDescent="0.3">
@@ -15546,7 +15549,7 @@
         <v>1344</v>
       </c>
       <c r="I412" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="413" spans="1:9" x14ac:dyDescent="0.3">
@@ -15575,7 +15578,7 @@
         <v>1344</v>
       </c>
       <c r="I413" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.3">
@@ -15604,7 +15607,7 @@
         <v>1344</v>
       </c>
       <c r="I414" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="415" spans="1:9" x14ac:dyDescent="0.3">
@@ -15630,7 +15633,7 @@
         <v>1344</v>
       </c>
       <c r="I415" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="416" spans="1:9" x14ac:dyDescent="0.3">
@@ -15659,7 +15662,7 @@
         <v>1345</v>
       </c>
       <c r="I416" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="417" spans="1:9" x14ac:dyDescent="0.3">
@@ -15688,7 +15691,7 @@
         <v>1345</v>
       </c>
       <c r="I417" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="418" spans="1:9" x14ac:dyDescent="0.3">
@@ -15714,7 +15717,7 @@
         <v>1267</v>
       </c>
       <c r="I418" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="419" spans="1:9" x14ac:dyDescent="0.3">
@@ -15740,7 +15743,7 @@
         <v>1267</v>
       </c>
       <c r="I419" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="420" spans="1:9" x14ac:dyDescent="0.3">
@@ -15766,7 +15769,7 @@
         <v>1267</v>
       </c>
       <c r="I420" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="421" spans="1:9" x14ac:dyDescent="0.3">
@@ -15789,10 +15792,10 @@
         <v>943</v>
       </c>
       <c r="H421" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
       <c r="I421" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="422" spans="1:9" x14ac:dyDescent="0.3">
@@ -15818,7 +15821,7 @@
         <v>1346</v>
       </c>
       <c r="I422" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.3">
@@ -15844,7 +15847,7 @@
         <v>1347</v>
       </c>
       <c r="I423" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.3">
@@ -15870,7 +15873,7 @@
         <v>1267</v>
       </c>
       <c r="I424" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="425" spans="1:9" x14ac:dyDescent="0.3">
@@ -15896,7 +15899,7 @@
         <v>1267</v>
       </c>
       <c r="I425" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.3">
@@ -15919,10 +15922,10 @@
         <v>1223</v>
       </c>
       <c r="H426" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
       <c r="I426" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -15945,10 +15948,10 @@
         <v>1224</v>
       </c>
       <c r="H427" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I427" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="428" spans="1:9" x14ac:dyDescent="0.3">
@@ -15971,10 +15974,10 @@
         <v>1187</v>
       </c>
       <c r="H428" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I428" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.3">
@@ -15997,10 +16000,10 @@
         <v>1225</v>
       </c>
       <c r="H429" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I429" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="430" spans="1:9" x14ac:dyDescent="0.3">
@@ -16023,10 +16026,10 @@
         <v>1226</v>
       </c>
       <c r="H430" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I430" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="431" spans="1:9" x14ac:dyDescent="0.3">
@@ -16049,10 +16052,10 @@
         <v>1227</v>
       </c>
       <c r="H431" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I431" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="432" spans="1:9" x14ac:dyDescent="0.3">
@@ -16075,10 +16078,10 @@
         <v>1228</v>
       </c>
       <c r="H432" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I432" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="433" spans="1:10" x14ac:dyDescent="0.3">
@@ -16101,10 +16104,10 @@
         <v>1229</v>
       </c>
       <c r="H433" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="I433" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="434" spans="1:10" x14ac:dyDescent="0.3">
@@ -16130,10 +16133,10 @@
         <v>1348</v>
       </c>
       <c r="I434" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J434" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="435" spans="1:10" x14ac:dyDescent="0.3">
@@ -16159,10 +16162,10 @@
         <v>1348</v>
       </c>
       <c r="I435" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J435" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.3">
@@ -16188,10 +16191,10 @@
         <v>1348</v>
       </c>
       <c r="I436" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J436" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="437" spans="1:10" x14ac:dyDescent="0.3">
@@ -16217,10 +16220,10 @@
         <v>1348</v>
       </c>
       <c r="I437" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J437" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="438" spans="1:10" x14ac:dyDescent="0.3">
@@ -16246,10 +16249,10 @@
         <v>1348</v>
       </c>
       <c r="I438" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J438" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="439" spans="1:10" x14ac:dyDescent="0.3">
@@ -16275,10 +16278,10 @@
         <v>1348</v>
       </c>
       <c r="I439" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="J439" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="440" spans="1:10" x14ac:dyDescent="0.3">
@@ -16304,7 +16307,7 @@
         <v>1349</v>
       </c>
       <c r="I440" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="441" spans="1:10" x14ac:dyDescent="0.3">
@@ -16330,7 +16333,7 @@
         <v>1350</v>
       </c>
       <c r="I441" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="442" spans="1:10" x14ac:dyDescent="0.3">
@@ -16356,7 +16359,7 @@
         <v>1351</v>
       </c>
       <c r="I442" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="443" spans="1:10" x14ac:dyDescent="0.3">
@@ -16385,7 +16388,7 @@
         <v>1352</v>
       </c>
       <c r="I443" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="444" spans="1:10" x14ac:dyDescent="0.3">
@@ -16411,7 +16414,7 @@
         <v>1352</v>
       </c>
       <c r="I444" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="445" spans="1:10" x14ac:dyDescent="0.3">
@@ -16437,7 +16440,7 @@
         <v>1352</v>
       </c>
       <c r="I445" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="446" spans="1:10" x14ac:dyDescent="0.3">
@@ -16463,7 +16466,7 @@
         <v>1352</v>
       </c>
       <c r="I446" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="447" spans="1:10" x14ac:dyDescent="0.3">
@@ -16489,7 +16492,7 @@
         <v>1352</v>
       </c>
       <c r="I447" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="448" spans="1:10" x14ac:dyDescent="0.3">
@@ -16515,7 +16518,7 @@
         <v>1353</v>
       </c>
       <c r="I448" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="449" spans="1:9" x14ac:dyDescent="0.3">
@@ -16541,7 +16544,7 @@
         <v>1353</v>
       </c>
       <c r="I449" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="450" spans="1:9" x14ac:dyDescent="0.3">
@@ -16567,7 +16570,7 @@
         <v>1353</v>
       </c>
       <c r="I450" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="451" spans="1:9" x14ac:dyDescent="0.3">
@@ -16593,7 +16596,7 @@
         <v>1354</v>
       </c>
       <c r="I451" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.3">
@@ -16619,7 +16622,7 @@
         <v>1355</v>
       </c>
       <c r="I452" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="453" spans="1:9" x14ac:dyDescent="0.3">
@@ -16645,7 +16648,7 @@
         <v>1356</v>
       </c>
       <c r="I453" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="454" spans="1:9" x14ac:dyDescent="0.3">
@@ -16671,7 +16674,7 @@
         <v>1356</v>
       </c>
       <c r="I454" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="455" spans="1:9" x14ac:dyDescent="0.3">
@@ -16697,7 +16700,7 @@
         <v>1356</v>
       </c>
       <c r="I455" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="456" spans="1:9" x14ac:dyDescent="0.3">
@@ -16723,7 +16726,7 @@
         <v>1357</v>
       </c>
       <c r="I456" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="457" spans="1:9" x14ac:dyDescent="0.3">
@@ -16749,7 +16752,7 @@
         <v>1357</v>
       </c>
       <c r="I457" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="458" spans="1:9" x14ac:dyDescent="0.3">
@@ -16775,7 +16778,7 @@
         <v>1357</v>
       </c>
       <c r="I458" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="459" spans="1:9" x14ac:dyDescent="0.3">
@@ -16801,7 +16804,7 @@
         <v>1357</v>
       </c>
       <c r="I459" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="460" spans="1:9" x14ac:dyDescent="0.3">
@@ -16827,7 +16830,7 @@
         <v>1357</v>
       </c>
       <c r="I460" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="461" spans="1:9" x14ac:dyDescent="0.3">
@@ -16853,7 +16856,7 @@
         <v>1357</v>
       </c>
       <c r="I461" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="462" spans="1:9" x14ac:dyDescent="0.3">
@@ -16879,7 +16882,7 @@
         <v>1358</v>
       </c>
       <c r="I462" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="463" spans="1:9" x14ac:dyDescent="0.3">
@@ -16905,7 +16908,7 @@
         <v>1359</v>
       </c>
       <c r="I463" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="464" spans="1:9" x14ac:dyDescent="0.3">
@@ -16931,7 +16934,7 @@
         <v>1360</v>
       </c>
       <c r="I464" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="465" spans="1:9" x14ac:dyDescent="0.3">
@@ -16957,7 +16960,7 @@
         <v>1311</v>
       </c>
       <c r="I465" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="466" spans="1:9" x14ac:dyDescent="0.3">
@@ -16983,7 +16986,7 @@
         <v>1312</v>
       </c>
       <c r="I466" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>